<commit_message>
CreateAnalysisReport working with minor bugs
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$B$8:$F$13</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Coordinates</t>
   </si>
@@ -57,16 +57,55 @@
     <t>Protocol Name</t>
   </si>
   <si>
-    <t>hrhrf</t>
-  </si>
-  <si>
-    <t>fh</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>5</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sample Study 1</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>plate</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Analysis 1</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>10ml</t>
+  </si>
+  <si>
+    <t>plasma</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>XYZ456</t>
+  </si>
+  <si>
+    <t>20ml</t>
+  </si>
+  <si>
+    <t>serum</t>
+  </si>
+  <si>
+    <t>13.0</t>
   </si>
 </sst>
 </file>
@@ -315,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,9 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -395,6 +431,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -433,15 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,10 +828,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G14"/>
+  <dimension ref="A2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -800,78 +848,82 @@
   <sheetData>
     <row r="2" spans="1:7" ht="49.5" customHeight="1">
       <c r="A2" s="4"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="42"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="28" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="18.75">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="42" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75">
+      <c r="B5" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="18" t="n">
+        <v>45488.0</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.5" customHeight="1">
+      <c r="B6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75">
-      <c r="B5" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1">
-      <c r="B6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="25.5" customHeight="1">
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="33" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="39" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -880,60 +932,75 @@
       <c r="F9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="33"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="34"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="3">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="2"/>
+      <c r="A12" s="3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Uploader added to InputAnalysisResult.java
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>Coordinates</t>
   </si>
@@ -63,22 +63,160 @@
     <t>Sample Study 2</t>
   </si>
   <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>2024-11-06_Analysis 4_nr_7_rt</t>
-  </si>
-  <si>
-    <t>nr</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Analysis 4</t>
-  </si>
-  <si>
-    <t>5000ßß000</t>
+    <t/>
+  </si>
+  <si>
+    <t>2024-07-28_Analysis 3__1_</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Analysis 3</t>
+  </si>
+  <si>
+    <t>5,2</t>
+  </si>
+  <si>
+    <t>ABCDEF123</t>
+  </si>
+  <si>
+    <t>100ml</t>
+  </si>
+  <si>
+    <t>plasma</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>rdherhya</t>
+  </si>
+  <si>
+    <t>700 µl</t>
+  </si>
+  <si>
+    <t>Serum</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>esdtgaewtz</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>sdgerh5</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>egaerzhrf</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>701 µl</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>702 µl</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>703 µl</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>704 µl</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>705 µl</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>706 µl</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>707 µl</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>708 µl</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>65656</t>
+  </si>
+  <si>
+    <t>709 µl</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>rtrer</t>
+  </si>
+  <si>
+    <t>710 µl</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>df43</t>
+  </si>
+  <si>
+    <t>711 µl</t>
   </si>
   <si>
     <t>A16</t>
@@ -88,12 +226,6 @@
   </si>
   <si>
     <t>712 µl</t>
-  </si>
-  <si>
-    <t>Serum</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>A17</t>
@@ -870,7 +1002,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G18"/>
+  <dimension ref="A2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -915,7 +1047,7 @@
       <c r="D4" s="15"/>
       <c r="E4" s="26"/>
       <c r="F4" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75">
@@ -924,7 +1056,7 @@
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="18" t="n">
-        <v>45602.0</v>
+        <v>45501.0</v>
       </c>
       <c r="E5" s="26"/>
       <c r="F5" s="27"/>
@@ -953,10 +1085,10 @@
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="25.5" customHeight="1">
       <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="12"/>
@@ -977,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="16.5" customHeight="1">
@@ -999,7 +1131,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1010,19 +1142,19 @@
         <v>11</v>
       </c>
       <c r="C12" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="F12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="G12" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13">
@@ -1031,19 +1163,19 @@
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>26</v>
-      </c>
       <c r="F13" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -1052,19 +1184,19 @@
       </c>
       <c r="B14" s="30"/>
       <c r="C14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -1073,19 +1205,19 @@
       </c>
       <c r="B15" s="30"/>
       <c r="C15" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -1094,19 +1226,19 @@
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -1115,19 +1247,19 @@
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -1136,19 +1268,355 @@
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="E19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F19" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>23</v>
+      <c r="D20" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>